<commit_message>
working in test data examples
</commit_message>
<xml_diff>
--- a/input/example_input_1.xlsx
+++ b/input/example_input_1.xlsx
@@ -1,21 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brsbio\OneDrive - UBC\varfilter_tag_amplicon_seq\input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_2F7DFDCE8F79A8D366075C52F3D2023480F5EA4A" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{F6A9ADAD-D6D8-4EF3-B291-81835084418A}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>VariantDescription</t>
+  </si>
+  <si>
+    <t>VAF</t>
+  </si>
+  <si>
+    <t>SupportingAmplicons</t>
+  </si>
+  <si>
+    <t>AmpliconProbeHits_1</t>
+  </si>
+  <si>
+    <t>AmpliconProbeHits_2</t>
+  </si>
+  <si>
+    <t>AmpliconProbeHits_3</t>
+  </si>
+  <si>
+    <t>Sample_001</t>
+  </si>
+  <si>
+    <t>VAR1</t>
+  </si>
+  <si>
+    <t>GENE1:c.1638G&gt;T|3:g.178936096G&gt;T</t>
+  </si>
+  <si>
+    <t>VAR2</t>
+  </si>
+  <si>
+    <t>GENE1:c.743G&gt;A|17:g.7579472G&gt;A</t>
+  </si>
+  <si>
+    <t>VAR3</t>
+  </si>
+  <si>
+    <t>GENE2:c.394C&gt;T|2:g.209113113C&gt;T</t>
+  </si>
+  <si>
+    <t>Sample_002</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +122,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -109,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +208,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +260,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,70 +453,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sample</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Variant</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>VariantDescription</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>VAF</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>SupportingAmplicons</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>AmpliconProbeHits_1</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>AmpliconProbeHits_2</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>AmpliconProbeHits_3</t>
-        </is>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Sample_001</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>VAR1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>GENE1:c.1638G&gt;T|3:g.178936096G&gt;T</t>
-        </is>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
       <c r="D2">
         <v>2.5</v>
@@ -431,24 +518,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sample_001</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>VAR2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>GENE1:c.743G&gt;A|17:g.7579472G&gt;A</t>
-        </is>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -463,53 +544,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Sample_001</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>VAR3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>GENE2:c.394C&gt;T|2:g.209113113C&gt;T</t>
-        </is>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H4">
-        <v>70</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Sample_002</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>VAR1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>GENE1:c.1638G&gt;T|3:g.178936096G&gt;T</t>
-        </is>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
       <c r="D5">
         <v>1.5</v>
@@ -527,24 +596,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Sample_002</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>VAR2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>GENE1:c.743G&gt;A|17:g.7579472G&gt;A</t>
-        </is>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -559,21 +622,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Sample_002</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>VAR3</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>GENE2:c.394C&gt;T|2:g.209113113C&gt;T</t>
-        </is>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
       </c>
       <c r="D7">
         <v>3</v>

</xml_diff>